<commit_message>
Updating Framework with headless and incognito mode functions
</commit_message>
<xml_diff>
--- a/SeleniumPOMTestNGFramework/src/test/resources/testdata/crmtestdata.xlsx
+++ b/SeleniumPOMTestNGFramework/src/test/resources/testdata/crmtestdata.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="contacts" sheetId="2" r:id="rId2"/>
+    <sheet name="forms" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>FirstName</t>
   </si>
@@ -56,19 +57,61 @@
   </si>
   <si>
     <t>Google</t>
+  </si>
+  <si>
+    <t>FormNameText</t>
+  </si>
+  <si>
+    <t>IntroText</t>
+  </si>
+  <si>
+    <t>CompleteText</t>
+  </si>
+  <si>
+    <t>TOM</t>
+  </si>
+  <si>
+    <t>Testing123</t>
+  </si>
+  <si>
+    <t>GSDFSDCSXCC</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Testing345</t>
+  </si>
+  <si>
+    <t>ASDASDASD</t>
+  </si>
+  <si>
+    <t>Mukta</t>
+  </si>
+  <si>
+    <t>Testing567</t>
+  </si>
+  <si>
+    <t>GDFSDFFFF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A3E3E"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -91,8 +134,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,7 +431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -441,4 +485,69 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>